<commit_message>
Vista Mayores_sub_cuenta v3 y Comprobantes procesados v1
</commit_message>
<xml_diff>
--- a/TEMP/EMPRESA_998/PLAN DE CUENTAS.xlsx
+++ b/TEMP/EMPRESA_998/PLAN DE CUENTAS.xlsx
@@ -42,7 +42,7 @@
         <sz val="7"/>
         <u val="none"/>
       </rPr>
-      <t xml:space="preserve">19:16
+      <t xml:space="preserve">22:23
 </t>
     </r>
     <r>
@@ -67,7 +67,7 @@
         <sz val="7"/>
         <u val="none"/>
       </rPr>
-      <t xml:space="preserve">07-11-2024
+      <t xml:space="preserve">20-11-2024
 </t>
     </r>
     <r>
@@ -12037,7 +12037,7 @@
               <sz val="7"/>
               <u val="none"/>
             </rPr>
-            <t xml:space="preserve">19:16
+            <t xml:space="preserve">22:23
 </t>
           </r>
           <r>
@@ -12062,7 +12062,7 @@
               <sz val="7"/>
               <u val="none"/>
             </rPr>
-            <t xml:space="preserve">07-11-2024
+            <t xml:space="preserve">20-11-2024
 </t>
           </r>
           <r>

</xml_diff>